<commit_message>
Aspirantes completos para el 22 de julio de 2024
</commit_message>
<xml_diff>
--- a/Julio/22 julio/ajalpan/PLANTILLA ASPIRANTES ITSSNA-24.xlsx
+++ b/Julio/22 julio/ajalpan/PLANTILLA ASPIRANTES ITSSNA-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxoC\OneDrive\Documents\EVALUATEC2024\Julio\22 julio\ajalpan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F39C41D-83CB-444B-8330-09EB7B15633B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFCA108-A53E-46D5-B148-4A52D360CA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1295,7 +1295,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1454,20 +1454,11 @@
     <xf numFmtId="18" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1480,7 +1471,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1497,6 +1487,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -1870,21 +1869,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="2" width="31.25" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.25" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="31.25" customWidth="1"/>
+    <col min="3" max="3" width="21.125" customWidth="1"/>
+    <col min="4" max="4" width="32.25" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="45.125" customWidth="1"/>
-    <col min="7" max="7" width="13.625" style="4" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
+    <col min="9" max="9" width="28.5" customWidth="1"/>
     <col min="10" max="10" width="22.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.375" customWidth="1"/>
@@ -1895,31 +1894,31 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="96" t="s">
+      <c r="K1" s="92" t="s">
         <v>315</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="95" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="96" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
         <v>316</v>
       </c>
-      <c r="L2" s="78"/>
+      <c r="L2" s="95"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L3" s="78"/>
+      <c r="L3" s="95"/>
     </row>
     <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2043,8 +2042,8 @@
       <c r="M6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
@@ -4046,7 +4045,7 @@
       <c r="D55" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="E55" s="95" t="s">
+      <c r="E55" s="91" t="s">
         <v>33</v>
       </c>
       <c r="F55" s="16" t="s">
@@ -4078,7 +4077,7 @@
       <c r="A56" s="7">
         <v>60</v>
       </c>
-      <c r="B56" s="79" t="s">
+      <c r="B56" s="76" t="s">
         <v>219</v>
       </c>
       <c r="C56" s="34" t="s">
@@ -4163,7 +4162,7 @@
       <c r="B58" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="C58" s="88" t="s">
+      <c r="C58" t="s">
         <v>235</v>
       </c>
       <c r="D58" s="67" t="s">
@@ -4406,13 +4405,13 @@
       <c r="A64" s="7">
         <v>91</v>
       </c>
-      <c r="B64" s="80" t="s">
+      <c r="B64" s="77" t="s">
         <v>312</v>
       </c>
-      <c r="C64" s="85" t="s">
+      <c r="C64" s="82" t="s">
         <v>313</v>
       </c>
-      <c r="D64" s="91" t="s">
+      <c r="D64" s="87" t="s">
         <v>314</v>
       </c>
       <c r="E64" s="56" t="s">
@@ -4775,7 +4774,7 @@
       <c r="A73" s="7">
         <v>74</v>
       </c>
-      <c r="B73" s="81" t="s">
+      <c r="B73" s="78" t="s">
         <v>261</v>
       </c>
       <c r="C73" s="34" t="s">
@@ -4939,13 +4938,13 @@
       <c r="A77" s="7">
         <v>90</v>
       </c>
-      <c r="B77" s="80" t="s">
+      <c r="B77" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="C77" s="85" t="s">
+      <c r="C77" s="82" t="s">
         <v>310</v>
       </c>
-      <c r="D77" s="91" t="s">
+      <c r="D77" s="87" t="s">
         <v>311</v>
       </c>
       <c r="E77" s="56" t="s">
@@ -5103,10 +5102,10 @@
       <c r="A81" s="48">
         <v>80</v>
       </c>
-      <c r="B81" s="83" t="s">
+      <c r="B81" s="80" t="s">
         <v>279</v>
       </c>
-      <c r="C81" s="88" t="s">
+      <c r="C81" t="s">
         <v>280</v>
       </c>
       <c r="D81" s="67" t="s">
@@ -5144,13 +5143,13 @@
       <c r="A82" s="48">
         <v>89</v>
       </c>
-      <c r="B82" s="84" t="s">
+      <c r="B82" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="C82" s="85" t="s">
+      <c r="C82" s="82" t="s">
         <v>307</v>
       </c>
-      <c r="D82" s="93" t="s">
+      <c r="D82" s="89" t="s">
         <v>308</v>
       </c>
       <c r="E82" s="56" t="s">
@@ -5308,7 +5307,7 @@
       <c r="A86" s="7">
         <v>66</v>
       </c>
-      <c r="B86" s="82" t="s">
+      <c r="B86" s="79" t="s">
         <v>237</v>
       </c>
       <c r="C86" s="33" t="s">
@@ -5475,10 +5474,10 @@
       <c r="B90" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="C90" s="90" t="s">
+      <c r="C90" s="86" t="s">
         <v>259</v>
       </c>
-      <c r="D90" s="94" t="s">
+      <c r="D90" s="90" t="s">
         <v>260</v>
       </c>
       <c r="E90" s="56" t="s">
@@ -5516,10 +5515,10 @@
       <c r="B91" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="C91" s="87" t="s">
+      <c r="C91" s="84" t="s">
         <v>265</v>
       </c>
-      <c r="D91" s="92" t="s">
+      <c r="D91" s="88" t="s">
         <v>266</v>
       </c>
       <c r="E91" s="56" t="s">
@@ -5598,7 +5597,7 @@
       <c r="B93" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C93" s="89" t="s">
+      <c r="C93" s="85" t="s">
         <v>295</v>
       </c>
       <c r="D93" s="68" t="s">
@@ -5639,7 +5638,7 @@
       <c r="B94" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="C94" s="86" t="s">
+      <c r="C94" s="83" t="s">
         <v>298</v>
       </c>
       <c r="D94" s="69" t="s">
@@ -5680,7 +5679,7 @@
       <c r="B95" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="C95" s="86" t="s">
+      <c r="C95" s="83" t="s">
         <v>304</v>
       </c>
       <c r="D95" s="69" t="s">

</xml_diff>